<commit_message>
aggiornati i calcoli su lab10 e lab20
</commit_message>
<xml_diff>
--- a/PROGETTO_PROLOG/Grafici prolog.xlsx
+++ b/PROGETTO_PROLOG/Grafici prolog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toby/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toby/Developing/Esercizi-IA-Lab/PROGETTO_PROLOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5080" yWindow="-21140" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="-5360" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mondo blocchi 1 - Profondita su" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="11">
   <si>
     <t>Profondita su grafo</t>
   </si>
@@ -630,11 +630,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2117816592"/>
-        <c:axId val="2117839536"/>
+        <c:axId val="2127805824"/>
+        <c:axId val="2127809616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117816592"/>
+        <c:axId val="2127805824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +677,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117839536"/>
+        <c:crossAx val="2127809616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -685,7 +685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117839536"/>
+        <c:axId val="2127809616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117816592"/>
+        <c:crossAx val="2127805824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,7 +861,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -995,7 +994,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1084,11 +1082,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2138661888"/>
-        <c:axId val="2138665376"/>
+        <c:axId val="-2136618992"/>
+        <c:axId val="-2136615504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2138661888"/>
+        <c:axId val="-2136618992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1129,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138665376"/>
+        <c:crossAx val="-2136615504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1139,7 +1137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138665376"/>
+        <c:axId val="-2136615504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1188,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138661888"/>
+        <c:crossAx val="-2136618992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1370,13 +1368,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15.0</c:v>
@@ -1385,10 +1383,10 @@
                   <c:v>1726.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>255.0</c:v>
+                  <c:v>290.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1507,22 +1505,22 @@
                   <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1538,11 +1536,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2138714432"/>
-        <c:axId val="2138717920"/>
+        <c:axId val="2130276960"/>
+        <c:axId val="2130239680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2138714432"/>
+        <c:axId val="2130276960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,7 +1583,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138717920"/>
+        <c:crossAx val="2130239680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1593,7 +1591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138717920"/>
+        <c:axId val="2130239680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,7 +1642,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138714432"/>
+        <c:crossAx val="2130276960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1830,16 +1828,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>191.0</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -1992,11 +1990,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2138767024"/>
-        <c:axId val="2138770512"/>
+        <c:axId val="2130349984"/>
+        <c:axId val="2130353472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2138767024"/>
+        <c:axId val="2130349984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2039,7 +2037,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138770512"/>
+        <c:crossAx val="2130353472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2047,7 +2045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138770512"/>
+        <c:axId val="2130353472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2096,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138767024"/>
+        <c:crossAx val="2130349984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5712,7 +5710,7 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -6302,11 +6300,11 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6343,13 +6341,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="16">
-        <v>15</v>
-      </c>
-      <c r="C2" s="16">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D2" s="16">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="E2" s="16">
         <v>15</v>
@@ -6358,10 +6356,10 @@
         <v>1726</v>
       </c>
       <c r="G2" s="16">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" s="16">
-        <v>255</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6372,22 +6370,22 @@
         <v>48</v>
       </c>
       <c r="C3" s="14">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="D3" s="14">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E3" s="14">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F3" s="14">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="G3" s="14">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="H3" s="14">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6598,10 +6596,10 @@
   <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6644,16 +6642,16 @@
         <v>9</v>
       </c>
       <c r="D2" s="11">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="11">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="5">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
aggiornamenti ad A* e a tutti i file per l'esame di Settembre
</commit_message>
<xml_diff>
--- a/PROGETTO_PROLOG/Grafici prolog.xlsx
+++ b/PROGETTO_PROLOG/Grafici prolog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5360" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mondo blocchi 1 - Profondita su" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
                   <c:v>263.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>986.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>248.0</c:v>
@@ -630,11 +630,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2127805824"/>
-        <c:axId val="2127809616"/>
+        <c:axId val="-2139828432"/>
+        <c:axId val="-2139824992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127805824"/>
+        <c:axId val="-2139828432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +677,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127809616"/>
+        <c:crossAx val="-2139824992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -685,7 +685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127809616"/>
+        <c:axId val="-2139824992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127805824"/>
+        <c:crossAx val="-2139828432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,6 +861,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -994,6 +995,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1082,11 +1084,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2136618992"/>
-        <c:axId val="-2136615504"/>
+        <c:axId val="-2139808512"/>
+        <c:axId val="-2139805072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2136618992"/>
+        <c:axId val="-2139808512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1131,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136615504"/>
+        <c:crossAx val="-2139805072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1137,7 +1139,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136615504"/>
+        <c:axId val="-2139805072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,7 +1190,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136618992"/>
+        <c:crossAx val="-2139808512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1374,19 +1376,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>190.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1726.0</c:v>
+                  <c:v>1217.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>290.0</c:v>
+                  <c:v>272.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1502,25 +1504,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>48.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1536,11 +1538,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2130276960"/>
-        <c:axId val="2130239680"/>
+        <c:axId val="-2112407232"/>
+        <c:axId val="-2112402000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130276960"/>
+        <c:axId val="-2112407232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,7 +1585,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130239680"/>
+        <c:crossAx val="-2112402000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1591,7 +1593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130239680"/>
+        <c:axId val="-2112402000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1644,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130276960"/>
+        <c:crossAx val="-2112407232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,7 +1839,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -1990,11 +1992,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2130349984"/>
-        <c:axId val="2130353472"/>
+        <c:axId val="-2110089472"/>
+        <c:axId val="-2110085904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130349984"/>
+        <c:axId val="-2110089472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,7 +2039,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130353472"/>
+        <c:crossAx val="-2110085904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2045,7 +2047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130353472"/>
+        <c:axId val="-2110085904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2096,7 +2098,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130349984"/>
+        <c:crossAx val="-2110089472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5711,10 +5713,10 @@
   <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5766,7 +5768,7 @@
         <v>263</v>
       </c>
       <c r="G2" s="16">
-        <v>986</v>
+        <v>70</v>
       </c>
       <c r="H2" s="16">
         <v>248</v>
@@ -6005,8 +6007,8 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
@@ -6300,8 +6302,8 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
@@ -6347,19 +6349,19 @@
         <v>9</v>
       </c>
       <c r="D2" s="16">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="E2" s="16">
         <v>15</v>
       </c>
       <c r="F2" s="16">
-        <v>1726</v>
+        <v>1217</v>
       </c>
       <c r="G2" s="16">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H2" s="16">
-        <v>290</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6367,25 +6369,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="14">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="14">
         <v>0</v>
       </c>
       <c r="D3" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6596,10 +6598,10 @@
   <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6651,7 +6653,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="5">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>9</v>

</xml_diff>